<commit_message>
Updated the last aluminum to even higher in case that's the real value
</commit_message>
<xml_diff>
--- a/data/attenuation.xlsx
+++ b/data/attenuation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhafn\PHY 451\PHY451-GammaRay\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16B58BAE-EF50-435F-BEA5-DE3D7B328B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D8445A-2E4F-4DAF-A170-BEBBDF4FBD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="1485" windowWidth="23595" windowHeight="19500" xr2:uid="{9168C447-9965-4F60-AF95-BACA57047A19}"/>
+    <workbookView xWindow="18570" yWindow="1170" windowWidth="23595" windowHeight="19500" xr2:uid="{9168C447-9965-4F60-AF95-BACA57047A19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,8 +730,7 @@
         <v>4</v>
       </c>
       <c r="B27">
-        <f>AVERAGE(4.627,4.651,4.599,4.637)+$B$26</f>
-        <v>9.2252499999999991</v>
+        <v>10.337249999999999</v>
       </c>
       <c r="C27">
         <v>80</v>
@@ -742,8 +741,7 @@
         <v>4</v>
       </c>
       <c r="B28">
-        <f t="shared" ref="B28:B30" si="6">AVERAGE(4.627,4.651,4.599,4.637)+$B$26</f>
-        <v>9.2252499999999991</v>
+        <v>10.337249999999999</v>
       </c>
       <c r="C28">
         <v>66</v>
@@ -754,8 +752,7 @@
         <v>4</v>
       </c>
       <c r="B29">
-        <f t="shared" si="6"/>
-        <v>9.2252499999999991</v>
+        <v>10.337249999999999</v>
       </c>
       <c r="C29">
         <v>74</v>
@@ -766,8 +763,7 @@
         <v>4</v>
       </c>
       <c r="B30">
-        <f t="shared" si="6"/>
-        <v>9.2252499999999991</v>
+        <v>10.337249999999999</v>
       </c>
       <c r="C30">
         <v>62</v>

</xml_diff>

<commit_message>
Rolling back to old value for aluminum's last thickness
</commit_message>
<xml_diff>
--- a/data/attenuation.xlsx
+++ b/data/attenuation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhafn\PHY 451\PHY451-GammaRay\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D8445A-2E4F-4DAF-A170-BEBBDF4FBD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3930CFC-76B1-4EF4-A2CA-798181B7859D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18570" yWindow="1170" windowWidth="23595" windowHeight="19500" xr2:uid="{9168C447-9965-4F60-AF95-BACA57047A19}"/>
   </bookViews>
@@ -408,7 +408,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,7 +730,7 @@
         <v>4</v>
       </c>
       <c r="B27">
-        <v>10.337249999999999</v>
+        <v>9.2252500000000008</v>
       </c>
       <c r="C27">
         <v>80</v>
@@ -741,7 +741,7 @@
         <v>4</v>
       </c>
       <c r="B28">
-        <v>10.337249999999999</v>
+        <v>9.2252500000000008</v>
       </c>
       <c r="C28">
         <v>66</v>
@@ -752,7 +752,7 @@
         <v>4</v>
       </c>
       <c r="B29">
-        <v>10.337249999999999</v>
+        <v>9.2252500000000008</v>
       </c>
       <c r="C29">
         <v>74</v>
@@ -763,7 +763,7 @@
         <v>4</v>
       </c>
       <c r="B30">
-        <v>10.337249999999999</v>
+        <v>9.2252500000000008</v>
       </c>
       <c r="C30">
         <v>62</v>

</xml_diff>